<commit_message>
removed filled vs template sub structure in test files dir
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/glioblastoma_100cells.xlsx
+++ b/examples/spreadsheets/current/filled/glioblastoma_100cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/Google Drive/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6C8D157C-E6C9-EA4F-BB8F-56630971F20E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DEFA8557-2C49-504C-9832-A33723CCDFC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27480" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -4585,8 +4585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4708,11 +4708,11 @@
       <c r="C6" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>657</v>
-      </c>
       <c r="F6" s="5" t="s">
         <v>656</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -5811,7 +5811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6:L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>